<commit_message>
Test_Graz_OnTrain adding and modify previous functions
</commit_message>
<xml_diff>
--- a/Results_excel/Graz_dataset/Graz_CrossVal_OnTrain.xlsx
+++ b/Results_excel/Graz_dataset/Graz_CrossVal_OnTrain.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1383" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1783" uniqueCount="27">
   <si>
     <t>date</t>
   </si>
@@ -145,7 +145,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -561,13 +561,68 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>45412.474209394306</v>
+      </c>
+      <c r="B8" s="0">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="0">
+        <v>83.680555555555557</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0">
+        <v>2</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="0">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -983,13 +1038,68 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>45412.474235007976</v>
+      </c>
+      <c r="B8" s="0">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="0">
+        <v>81.25</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0">
+        <v>2</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="0">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1429,11 +1539,994 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>45412.474238290219</v>
+      </c>
+      <c r="B8" s="0">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="0">
+        <v>80.902777777777786</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0">
+        <v>2</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="0">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="true"/>
+    <col min="2" max="2" width="7.33203125" customWidth="true"/>
+    <col min="3" max="3" width="4.21875" customWidth="true"/>
+    <col min="4" max="4" width="4.6640625" customWidth="true"/>
+    <col min="5" max="5" width="10.33203125" customWidth="true"/>
+    <col min="6" max="6" width="9.5546875" customWidth="true"/>
+    <col min="7" max="7" width="9.33203125" customWidth="true"/>
+    <col min="8" max="8" width="14.21875" customWidth="true"/>
+    <col min="9" max="9" width="12.109375" customWidth="true"/>
+    <col min="10" max="10" width="9.6640625" customWidth="true"/>
+    <col min="11" max="11" width="8.88671875" customWidth="true"/>
+    <col min="12" max="12" width="8.6640625" customWidth="true"/>
+    <col min="13" max="13" width="13.5546875" customWidth="true"/>
+    <col min="14" max="14" width="11.44140625" customWidth="true"/>
+    <col min="15" max="15" width="2.5546875" customWidth="true"/>
+    <col min="16" max="16" width="8.88671875" customWidth="true"/>
+    <col min="17" max="17" width="9.77734375" customWidth="true"/>
+    <col min="18" max="18" width="6.109375" customWidth="true"/>
+    <col min="19" max="19" width="7" customWidth="true"/>
+    <col min="20" max="20" width="4" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>45411.725999631308</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M2" s="0">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0">
+        <v>2</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>45411.727779271365</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I3" s="0">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M3" s="0">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0">
+        <v>0</v>
+      </c>
+      <c r="O3" s="0">
+        <v>2</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>45411.739533348853</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="I4" s="0">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M4" s="0">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0">
+        <v>2</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>45411.750819024674</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.73611111111111105</v>
+      </c>
+      <c r="I5" s="0">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M5" s="0">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0">
+        <v>2</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>45411.753687906632</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.78240740740740733</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M6" s="0">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0">
+        <v>2</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>45412.474209267129</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0.78240740740740733</v>
+      </c>
+      <c r="I7" s="0">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0">
+        <v>2</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="0">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="true"/>
+    <col min="2" max="2" width="7.33203125" customWidth="true"/>
+    <col min="3" max="3" width="4.21875" customWidth="true"/>
+    <col min="4" max="4" width="4.6640625" customWidth="true"/>
+    <col min="5" max="5" width="10.33203125" customWidth="true"/>
+    <col min="6" max="6" width="9.5546875" customWidth="true"/>
+    <col min="7" max="7" width="9.33203125" customWidth="true"/>
+    <col min="8" max="8" width="14.21875" customWidth="true"/>
+    <col min="9" max="9" width="12.109375" customWidth="true"/>
+    <col min="10" max="10" width="9.6640625" customWidth="true"/>
+    <col min="11" max="11" width="8.88671875" customWidth="true"/>
+    <col min="12" max="12" width="8.6640625" customWidth="true"/>
+    <col min="13" max="13" width="13.5546875" customWidth="true"/>
+    <col min="14" max="14" width="11.44140625" customWidth="true"/>
+    <col min="15" max="15" width="2.5546875" customWidth="true"/>
+    <col min="16" max="16" width="8.88671875" customWidth="true"/>
+    <col min="17" max="17" width="9.77734375" customWidth="true"/>
+    <col min="18" max="18" width="6.109375" customWidth="true"/>
+    <col min="19" max="19" width="7" customWidth="true"/>
+    <col min="20" max="20" width="4" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>45411.726000113267</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M2" s="0">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0">
+        <v>2</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>45411.727780182788</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I3" s="0">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M3" s="0">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0">
+        <v>0</v>
+      </c>
+      <c r="O3" s="0">
+        <v>2</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>45411.739534328532</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0.64814814814814803</v>
+      </c>
+      <c r="I4" s="0">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M4" s="0">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0">
+        <v>2</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>45411.750819911671</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.73148148148148151</v>
+      </c>
+      <c r="I5" s="0">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M5" s="0">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0">
+        <v>2</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>45411.753688919598</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M6" s="0">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0">
+        <v>2</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>45412.474234987858</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="I7" s="0">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0">
+        <v>2</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="0">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
@@ -1527,818 +2620,6 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>45411.725999631308</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="0">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H2" s="0">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="I2" s="0">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L2" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M2" s="0">
-        <v>0</v>
-      </c>
-      <c r="N2" s="0">
-        <v>0</v>
-      </c>
-      <c r="O2" s="0">
-        <v>2</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>45411.727779271365</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="0">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H3" s="0">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="I3" s="0">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L3" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M3" s="0">
-        <v>0</v>
-      </c>
-      <c r="N3" s="0">
-        <v>0</v>
-      </c>
-      <c r="O3" s="0">
-        <v>2</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>45411.739533348853</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="0">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H4" s="0">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="I4" s="0">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M4" s="0">
-        <v>0</v>
-      </c>
-      <c r="N4" s="0">
-        <v>0</v>
-      </c>
-      <c r="O4" s="0">
-        <v>2</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>45411.750819024674</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="0">
-        <v>8</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H5" s="0">
-        <v>0.73611111111111105</v>
-      </c>
-      <c r="I5" s="0">
-        <v>0</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L5" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M5" s="0">
-        <v>0</v>
-      </c>
-      <c r="N5" s="0">
-        <v>0</v>
-      </c>
-      <c r="O5" s="0">
-        <v>2</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>45411.753687906632</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="0">
-        <v>9</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H6" s="0">
-        <v>0.78240740740740733</v>
-      </c>
-      <c r="I6" s="0">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L6" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M6" s="0">
-        <v>0</v>
-      </c>
-      <c r="N6" s="0">
-        <v>0</v>
-      </c>
-      <c r="O6" s="0">
-        <v>2</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T6" s="0">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="true"/>
-    <col min="2" max="2" width="7.33203125" customWidth="true"/>
-    <col min="3" max="3" width="4.21875" customWidth="true"/>
-    <col min="4" max="4" width="4.6640625" customWidth="true"/>
-    <col min="5" max="5" width="10.33203125" customWidth="true"/>
-    <col min="6" max="6" width="9.5546875" customWidth="true"/>
-    <col min="7" max="7" width="9.33203125" customWidth="true"/>
-    <col min="8" max="8" width="14.21875" customWidth="true"/>
-    <col min="9" max="9" width="12.109375" customWidth="true"/>
-    <col min="10" max="10" width="9.6640625" customWidth="true"/>
-    <col min="11" max="11" width="8.88671875" customWidth="true"/>
-    <col min="12" max="12" width="8.6640625" customWidth="true"/>
-    <col min="13" max="13" width="13.5546875" customWidth="true"/>
-    <col min="14" max="14" width="11.44140625" customWidth="true"/>
-    <col min="15" max="15" width="2.5546875" customWidth="true"/>
-    <col min="16" max="16" width="8.88671875" customWidth="true"/>
-    <col min="17" max="17" width="9.77734375" customWidth="true"/>
-    <col min="18" max="18" width="6.109375" customWidth="true"/>
-    <col min="19" max="19" width="7" customWidth="true"/>
-    <col min="20" max="20" width="4" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>45411.726000113267</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="0">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H2" s="0">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="I2" s="0">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L2" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M2" s="0">
-        <v>0</v>
-      </c>
-      <c r="N2" s="0">
-        <v>0</v>
-      </c>
-      <c r="O2" s="0">
-        <v>2</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>45411.727780182788</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="0">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H3" s="0">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="I3" s="0">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L3" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M3" s="0">
-        <v>0</v>
-      </c>
-      <c r="N3" s="0">
-        <v>0</v>
-      </c>
-      <c r="O3" s="0">
-        <v>2</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>45411.739534328532</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="0">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H4" s="0">
-        <v>0.64814814814814803</v>
-      </c>
-      <c r="I4" s="0">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M4" s="0">
-        <v>0</v>
-      </c>
-      <c r="N4" s="0">
-        <v>0</v>
-      </c>
-      <c r="O4" s="0">
-        <v>2</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>45411.750819911671</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="0">
-        <v>8</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H5" s="0">
-        <v>0.73148148148148151</v>
-      </c>
-      <c r="I5" s="0">
-        <v>0</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L5" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M5" s="0">
-        <v>0</v>
-      </c>
-      <c r="N5" s="0">
-        <v>0</v>
-      </c>
-      <c r="O5" s="0">
-        <v>2</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>45411.753688919591</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="0">
-        <v>9</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="H6" s="0">
-        <v>0.74999999999999989</v>
-      </c>
-      <c r="I6" s="0">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="L6" s="0">
-        <v>2.5</v>
-      </c>
-      <c r="M6" s="0">
-        <v>0</v>
-      </c>
-      <c r="N6" s="0">
-        <v>0</v>
-      </c>
-      <c r="O6" s="0">
-        <v>2</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="T6" s="0">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="true"/>
-    <col min="2" max="2" width="7.33203125" customWidth="true"/>
-    <col min="3" max="3" width="4.21875" customWidth="true"/>
-    <col min="4" max="4" width="4.6640625" customWidth="true"/>
-    <col min="5" max="5" width="10.33203125" customWidth="true"/>
-    <col min="6" max="6" width="9.5546875" customWidth="true"/>
-    <col min="7" max="7" width="9.33203125" customWidth="true"/>
-    <col min="8" max="8" width="14.21875" customWidth="true"/>
-    <col min="9" max="9" width="12.109375" customWidth="true"/>
-    <col min="10" max="10" width="9.6640625" customWidth="true"/>
-    <col min="11" max="11" width="8.88671875" customWidth="true"/>
-    <col min="12" max="12" width="8.6640625" customWidth="true"/>
-    <col min="13" max="13" width="13.5546875" customWidth="true"/>
-    <col min="14" max="14" width="11.44140625" customWidth="true"/>
-    <col min="15" max="15" width="2.5546875" customWidth="true"/>
-    <col min="16" max="16" width="8.88671875" customWidth="true"/>
-    <col min="17" max="17" width="9.77734375" customWidth="true"/>
-    <col min="18" max="18" width="6.109375" customWidth="true"/>
-    <col min="19" max="19" width="7" customWidth="true"/>
-    <col min="20" max="20" width="4" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
         <v>45411.727781152244</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2525,7 +2806,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>45411.753690099009</v>
+        <v>45411.753690099002</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>26</v>
@@ -2582,6 +2863,64 @@
         <v>23</v>
       </c>
       <c r="T5" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>45412.474238276969</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.74537037037037035</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0">
+        <v>2</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>